<commit_message>
Add script, documentation and readme file
</commit_message>
<xml_diff>
--- a/Docks/ЛР1.xlsx
+++ b/Docks/ЛР1.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Алексей\Desktop\Random_number_generation\Docks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexp\OneDrive\Desktop\Random_number_generation\Docks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77652C92-F268-497D-B1FD-7AE8805C63D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9106511-337A-4AA1-ABA2-B93BAA850ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Промежуток</t>
   </si>
@@ -42,98 +48,110 @@
     <t>0.0000</t>
   </si>
   <si>
-    <t>0.0333</t>
-  </si>
-  <si>
-    <t>0.0667</t>
-  </si>
-  <si>
-    <t>0.1000</t>
-  </si>
-  <si>
-    <t>0.1333</t>
-  </si>
-  <si>
-    <t>0.1667</t>
-  </si>
-  <si>
-    <t>0.2000</t>
-  </si>
-  <si>
-    <t>0.2333</t>
-  </si>
-  <si>
-    <t>0.2667</t>
-  </si>
-  <si>
-    <t>0.3000</t>
-  </si>
-  <si>
-    <t>0.3333</t>
-  </si>
-  <si>
-    <t>0.3667</t>
-  </si>
-  <si>
-    <t>0.4000</t>
-  </si>
-  <si>
-    <t>0.4333</t>
-  </si>
-  <si>
-    <t>0.4667</t>
-  </si>
-  <si>
-    <t>0.5000</t>
-  </si>
-  <si>
-    <t>0.5333</t>
-  </si>
-  <si>
-    <t>0.5667</t>
-  </si>
-  <si>
-    <t>0.6000</t>
-  </si>
-  <si>
-    <t>0.6333</t>
-  </si>
-  <si>
-    <t>0.6667</t>
-  </si>
-  <si>
-    <t>0.7000</t>
-  </si>
-  <si>
-    <t>0.7333</t>
-  </si>
-  <si>
-    <t>0.7667</t>
-  </si>
-  <si>
-    <t>0.8000</t>
-  </si>
-  <si>
-    <t>0.8333</t>
-  </si>
-  <si>
-    <t>0.8667</t>
-  </si>
-  <si>
-    <t>0.9000</t>
-  </si>
-  <si>
-    <t>0.9333</t>
-  </si>
-  <si>
-    <t>0.9667</t>
+    <t>Критерий χ2:</t>
+  </si>
+  <si>
+    <t>0.0323</t>
+  </si>
+  <si>
+    <t>0.0645</t>
+  </si>
+  <si>
+    <t>0.0968</t>
+  </si>
+  <si>
+    <t>0.1290</t>
+  </si>
+  <si>
+    <t>0.1613</t>
+  </si>
+  <si>
+    <t>0.1935</t>
+  </si>
+  <si>
+    <t>0.2258</t>
+  </si>
+  <si>
+    <t>0.2581</t>
+  </si>
+  <si>
+    <t>0.2903</t>
+  </si>
+  <si>
+    <t>0.3226</t>
+  </si>
+  <si>
+    <t>0.3548</t>
+  </si>
+  <si>
+    <t>0.3871</t>
+  </si>
+  <si>
+    <t>0.4194</t>
+  </si>
+  <si>
+    <t>0.4516</t>
+  </si>
+  <si>
+    <t>0.4839</t>
+  </si>
+  <si>
+    <t>0.5161</t>
+  </si>
+  <si>
+    <t>0.5484</t>
+  </si>
+  <si>
+    <t>0.5806</t>
+  </si>
+  <si>
+    <t>0.6129</t>
+  </si>
+  <si>
+    <t>0.6452</t>
+  </si>
+  <si>
+    <t>0.6774</t>
+  </si>
+  <si>
+    <t>0.7097</t>
+  </si>
+  <si>
+    <t>0.7419</t>
+  </si>
+  <si>
+    <t>0.7742</t>
+  </si>
+  <si>
+    <t>0.8065</t>
+  </si>
+  <si>
+    <t>0.8387</t>
+  </si>
+  <si>
+    <t>0.8710</t>
+  </si>
+  <si>
+    <t>0.9032</t>
+  </si>
+  <si>
+    <t>0.9355</t>
+  </si>
+  <si>
+    <t>0.9677</t>
+  </si>
+  <si>
+    <t>Степеней свободы:</t>
+  </si>
+  <si>
+    <t>22.1442</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,16 +159,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -158,13 +196,193 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -295,96 +513,99 @@
               </c:extLst>
               <c:f>Sheet1!$A$2:$A$1048576</c:f>
               <c:strCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0.0000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0333</c:v>
+                  <c:v>0.0323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0667</c:v>
+                  <c:v>0.0645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1000</c:v>
+                  <c:v>0.0968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1333</c:v>
+                  <c:v>0.1290</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1667</c:v>
+                  <c:v>0.1613</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2000</c:v>
+                  <c:v>0.1935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2333</c:v>
+                  <c:v>0.2258</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2667</c:v>
+                  <c:v>0.2581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3000</c:v>
+                  <c:v>0.2903</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3333</c:v>
+                  <c:v>0.3226</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3667</c:v>
+                  <c:v>0.3548</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.4000</c:v>
+                  <c:v>0.3871</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.4333</c:v>
+                  <c:v>0.4194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.4667</c:v>
+                  <c:v>0.4516</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5000</c:v>
+                  <c:v>0.4839</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.5333</c:v>
+                  <c:v>0.5161</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5667</c:v>
+                  <c:v>0.5484</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.6000</c:v>
+                  <c:v>0.5806</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.6333</c:v>
+                  <c:v>0.6129</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.6667</c:v>
+                  <c:v>0.6452</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.7000</c:v>
+                  <c:v>0.6774</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.7333</c:v>
+                  <c:v>0.7097</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.7667</c:v>
+                  <c:v>0.7419</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8000</c:v>
+                  <c:v>0.7742</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8333</c:v>
+                  <c:v>0.8065</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.8667</c:v>
+                  <c:v>0.8387</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.9000</c:v>
+                  <c:v>0.8710</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.9333</c:v>
+                  <c:v>0.9032</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.9667</c:v>
+                  <c:v>0.9355</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9677</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -403,91 +624,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>661</c:v>
+                  <c:v>644</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>678</c:v>
+                  <c:v>648</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>685</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>659</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>705</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>671</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>652</c:v>
+                  <c:v>619</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>666</c:v>
+                  <c:v>640</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>633</c:v>
+                  <c:v>628</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>702</c:v>
+                  <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>633</c:v>
+                  <c:v>646</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>628</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>656</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>664</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>643</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>670</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>687</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>668</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>648</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>687</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>692</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>640</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>671</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>683</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>709</c:v>
-                </c:pt>
                 <c:pt idx="20">
-                  <c:v>724</c:v>
+                  <c:v>696</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>646</c:v>
+                  <c:v>679</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>680</c:v>
+                  <c:v>629</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>625</c:v>
+                  <c:v>651</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>622</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>628</c:v>
+                  <c:v>604</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>685</c:v>
+                  <c:v>608</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>654</c:v>
+                  <c:v>667</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>648</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,96 +754,99 @@
               </c:extLst>
               <c:f>Sheet1!$A$2:$A$1048576</c:f>
               <c:strCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0.0000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0333</c:v>
+                  <c:v>0.0323</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0667</c:v>
+                  <c:v>0.0645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1000</c:v>
+                  <c:v>0.0968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1333</c:v>
+                  <c:v>0.1290</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1667</c:v>
+                  <c:v>0.1613</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2000</c:v>
+                  <c:v>0.1935</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2333</c:v>
+                  <c:v>0.2258</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2667</c:v>
+                  <c:v>0.2581</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3000</c:v>
+                  <c:v>0.2903</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3333</c:v>
+                  <c:v>0.3226</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3667</c:v>
+                  <c:v>0.3548</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.4000</c:v>
+                  <c:v>0.3871</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.4333</c:v>
+                  <c:v>0.4194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.4667</c:v>
+                  <c:v>0.4516</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.5000</c:v>
+                  <c:v>0.4839</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.5333</c:v>
+                  <c:v>0.5161</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.5667</c:v>
+                  <c:v>0.5484</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.6000</c:v>
+                  <c:v>0.5806</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.6333</c:v>
+                  <c:v>0.6129</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.6667</c:v>
+                  <c:v>0.6452</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.7000</c:v>
+                  <c:v>0.6774</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.7333</c:v>
+                  <c:v>0.7097</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.7667</c:v>
+                  <c:v>0.7419</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.8000</c:v>
+                  <c:v>0.7742</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.8333</c:v>
+                  <c:v>0.8065</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.8667</c:v>
+                  <c:v>0.8387</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.9000</c:v>
+                  <c:v>0.8710</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.9333</c:v>
+                  <c:v>0.9032</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.9667</c:v>
+                  <c:v>0.9355</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.9677</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -641,91 +865,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>666</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -794,96 +1018,99 @@
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
-                      <c:ptCount val="30"/>
+                      <c:ptCount val="31"/>
                       <c:pt idx="0">
                         <c:v>0.0000</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.0333</c:v>
+                        <c:v>0.0323</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.0667</c:v>
+                        <c:v>0.0645</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.1000</c:v>
+                        <c:v>0.0968</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.1333</c:v>
+                        <c:v>0.1290</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.1667</c:v>
+                        <c:v>0.1613</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>0.2000</c:v>
+                        <c:v>0.1935</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>0.2333</c:v>
+                        <c:v>0.2258</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.2667</c:v>
+                        <c:v>0.2581</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.3000</c:v>
+                        <c:v>0.2903</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>0.3333</c:v>
+                        <c:v>0.3226</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>0.3667</c:v>
+                        <c:v>0.3548</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.4000</c:v>
+                        <c:v>0.3871</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>0.4333</c:v>
+                        <c:v>0.4194</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>0.4667</c:v>
+                        <c:v>0.4516</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>0.5000</c:v>
+                        <c:v>0.4839</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0.5333</c:v>
+                        <c:v>0.5161</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>0.5667</c:v>
+                        <c:v>0.5484</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>0.6000</c:v>
+                        <c:v>0.5806</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.6333</c:v>
+                        <c:v>0.6129</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>0.6667</c:v>
+                        <c:v>0.6452</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>0.7000</c:v>
+                        <c:v>0.6774</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>0.7333</c:v>
+                        <c:v>0.7097</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>0.7667</c:v>
+                        <c:v>0.7419</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>0.8000</c:v>
+                        <c:v>0.7742</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>0.8333</c:v>
+                        <c:v>0.8065</c:v>
                       </c:pt>
                       <c:pt idx="26">
-                        <c:v>0.8667</c:v>
+                        <c:v>0.8387</c:v>
                       </c:pt>
                       <c:pt idx="27">
-                        <c:v>0.9000</c:v>
+                        <c:v>0.8710</c:v>
                       </c:pt>
                       <c:pt idx="28">
-                        <c:v>0.9333</c:v>
+                        <c:v>0.9032</c:v>
                       </c:pt>
                       <c:pt idx="29">
-                        <c:v>0.9667</c:v>
+                        <c:v>0.9355</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0.9677</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -1742,15 +1969,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
+      <xdr:colOff>36283</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>27215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>573127</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>136769</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2041,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,351 +2279,879 @@
     <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="31.109375" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>673</v>
-      </c>
-      <c r="C2" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="2">
+        <v>651</v>
+      </c>
+      <c r="C2" s="2">
+        <v>645</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>644</v>
+      </c>
+      <c r="C3" s="2">
+        <v>645</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>648</v>
+      </c>
+      <c r="C4" s="2">
+        <v>645</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>639</v>
+      </c>
+      <c r="C5" s="2">
+        <v>645</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>685</v>
+      </c>
+      <c r="C6" s="2">
+        <v>645</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>659</v>
+      </c>
+      <c r="C7" s="2">
+        <v>645</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>619</v>
+      </c>
+      <c r="C8" s="2">
+        <v>645</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>640</v>
+      </c>
+      <c r="C9" s="2">
+        <v>645</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2">
+        <v>628</v>
+      </c>
+      <c r="C10" s="2">
+        <v>645</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <v>657</v>
+      </c>
+      <c r="C11" s="2">
+        <v>645</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <v>646</v>
+      </c>
+      <c r="C12" s="2">
+        <v>645</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
+        <v>628</v>
+      </c>
+      <c r="C13" s="2">
+        <v>645</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
+        <v>656</v>
+      </c>
+      <c r="C14" s="2">
+        <v>645</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2">
+        <v>649</v>
+      </c>
+      <c r="C15" s="2">
+        <v>645</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2">
+        <v>642</v>
+      </c>
+      <c r="C16" s="2">
+        <v>645</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2">
+        <v>650</v>
+      </c>
+      <c r="C17" s="2">
+        <v>645</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2">
+        <v>664</v>
+      </c>
+      <c r="C18" s="2">
+        <v>645</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2">
+        <v>643</v>
+      </c>
+      <c r="C19" s="2">
+        <v>645</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2">
+        <v>642</v>
+      </c>
+      <c r="C20" s="2">
+        <v>645</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2">
+        <v>648</v>
+      </c>
+      <c r="C21" s="2">
+        <v>645</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>670</v>
+      </c>
+      <c r="C22" s="2">
+        <v>645</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2">
+        <v>696</v>
+      </c>
+      <c r="C23" s="2">
+        <v>645</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>679</v>
+      </c>
+      <c r="C24" s="2">
+        <v>645</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2">
+        <v>629</v>
+      </c>
+      <c r="C25" s="2">
+        <v>645</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2">
+        <v>651</v>
+      </c>
+      <c r="C26" s="2">
+        <v>645</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2">
+        <v>608</v>
+      </c>
+      <c r="C27" s="2">
+        <v>645</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2">
+        <v>604</v>
+      </c>
+      <c r="C28" s="2">
+        <v>645</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+    </row>
+    <row r="29" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2">
+        <v>608</v>
+      </c>
+      <c r="C29" s="2">
+        <v>645</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+    </row>
+    <row r="30" spans="1:18" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2">
+        <v>667</v>
+      </c>
+      <c r="C30" s="2">
+        <v>645</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+    </row>
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2">
+        <v>630</v>
+      </c>
+      <c r="C31" s="2">
+        <v>645</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>661</v>
-      </c>
-      <c r="C3" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>678</v>
-      </c>
-      <c r="C4" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>659</v>
-      </c>
-      <c r="C5" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>705</v>
-      </c>
-      <c r="C6" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>671</v>
-      </c>
-      <c r="C7" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>652</v>
-      </c>
-      <c r="C8" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>666</v>
-      </c>
-      <c r="C9" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>633</v>
-      </c>
-      <c r="C10" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
-        <v>702</v>
-      </c>
-      <c r="C11" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>633</v>
-      </c>
-      <c r="C12" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>670</v>
-      </c>
-      <c r="C13" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>687</v>
-      </c>
-      <c r="C14" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>668</v>
-      </c>
-      <c r="C15" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>648</v>
-      </c>
-      <c r="C16" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1">
-        <v>687</v>
-      </c>
-      <c r="C17" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1">
-        <v>692</v>
-      </c>
-      <c r="C18" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1">
-        <v>640</v>
-      </c>
-      <c r="C19" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
-        <v>671</v>
-      </c>
-      <c r="C20" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1">
-        <v>683</v>
-      </c>
-      <c r="C21" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
-        <v>709</v>
-      </c>
-      <c r="C22" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1">
-        <v>724</v>
-      </c>
-      <c r="C23" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1">
-        <v>646</v>
-      </c>
-      <c r="C24" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1">
-        <v>680</v>
-      </c>
-      <c r="C25" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1">
-        <v>625</v>
-      </c>
-      <c r="C26" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1">
-        <v>622</v>
-      </c>
-      <c r="C27" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1">
-        <v>628</v>
-      </c>
-      <c r="C28" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="E31" s="23"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="23"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K31" s="23"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="22">
         <v>30</v>
       </c>
-      <c r="B29" s="1">
-        <v>685</v>
-      </c>
-      <c r="C29" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1">
-        <v>654</v>
-      </c>
-      <c r="C30" s="1">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1">
-        <v>648</v>
-      </c>
-      <c r="C31" s="1">
-        <v>666</v>
-      </c>
+      <c r="N31" s="23"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+    </row>
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="14">
+        <v>620</v>
+      </c>
+      <c r="C32" s="14">
+        <v>645</v>
+      </c>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="26"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D31:F32"/>
+    <mergeCell ref="G31:I32"/>
+    <mergeCell ref="J31:L32"/>
+    <mergeCell ref="M31:O32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>